<commit_message>
New Load Test Suite Added
</commit_message>
<xml_diff>
--- a/LIMS User Details For Automation.xlsx
+++ b/LIMS User Details For Automation.xlsx
@@ -13,7 +13,7 @@
     <sheet name="RegistrationRole" sheetId="24" r:id="rId4"/>
     <sheet name="SampleRole" sheetId="6" r:id="rId5"/>
     <sheet name="StabilityRole" sheetId="7" r:id="rId6"/>
-    <sheet name="Sheet3" sheetId="26" r:id="rId7"/>
+    <sheet name="SampleRegistration" sheetId="26" r:id="rId7"/>
     <sheet name="MCRole" sheetId="8" r:id="rId8"/>
     <sheet name="CAPARole" sheetId="9" r:id="rId9"/>
     <sheet name="INVRole" sheetId="10" r:id="rId10"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="528" uniqueCount="236">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="534" uniqueCount="242">
   <si>
     <t>Location</t>
   </si>
@@ -658,70 +658,88 @@
     <t>TestName</t>
   </si>
   <si>
+    <t>RM Qualitative Test -2</t>
+  </si>
+  <si>
+    <t>RM Qualitative Test -1</t>
+  </si>
+  <si>
+    <t>RM Qualitative Test -3</t>
+  </si>
+  <si>
+    <t>RM Qualitative Test -4</t>
+  </si>
+  <si>
+    <t>RM Qualitative Test -5</t>
+  </si>
+  <si>
+    <t>RM Qualitative Test -6</t>
+  </si>
+  <si>
+    <t>RM Quantitative Test-1</t>
+  </si>
+  <si>
+    <t>RM Quantitative Test-2</t>
+  </si>
+  <si>
+    <t>RM Quantitative Test-3</t>
+  </si>
+  <si>
+    <t>RM Quantitative Test-4</t>
+  </si>
+  <si>
+    <t>RM Quantitative Test-5</t>
+  </si>
+  <si>
+    <t>RM Quantitative Test-6</t>
+  </si>
+  <si>
+    <t>Product_Code</t>
+  </si>
+  <si>
+    <t>Auto_Prod_1</t>
+  </si>
+  <si>
+    <t>Auto_Prod_2</t>
+  </si>
+  <si>
+    <t>Specification_Name</t>
+  </si>
+  <si>
+    <t>Auto_Spec_1</t>
+  </si>
+  <si>
+    <t>Auto_Spec_2</t>
+  </si>
+  <si>
+    <t>Plant-2</t>
+  </si>
+  <si>
     <t>Plant-2-QC</t>
   </si>
   <si>
+    <t>SMAUTO8</t>
+  </si>
+  <si>
+    <t>SM008</t>
+  </si>
+  <si>
+    <t>SMAUTO9</t>
+  </si>
+  <si>
+    <t>SM009</t>
+  </si>
+  <si>
+    <t>Plant-2-QA</t>
+  </si>
+  <si>
+    <t>REGAUTO5</t>
+  </si>
+  <si>
+    <t>REG005</t>
+  </si>
+  <si>
     <t>Plant-2-PF</t>
-  </si>
-  <si>
-    <t>Plant-2-QA</t>
-  </si>
-  <si>
-    <t>Plant-2</t>
-  </si>
-  <si>
-    <t>RM Qualitative Test -2</t>
-  </si>
-  <si>
-    <t>RM Qualitative Test -1</t>
-  </si>
-  <si>
-    <t>RM Qualitative Test -3</t>
-  </si>
-  <si>
-    <t>RM Qualitative Test -4</t>
-  </si>
-  <si>
-    <t>RM Qualitative Test -5</t>
-  </si>
-  <si>
-    <t>RM Qualitative Test -6</t>
-  </si>
-  <si>
-    <t>RM Quantitative Test-1</t>
-  </si>
-  <si>
-    <t>RM Quantitative Test-2</t>
-  </si>
-  <si>
-    <t>RM Quantitative Test-3</t>
-  </si>
-  <si>
-    <t>RM Quantitative Test-4</t>
-  </si>
-  <si>
-    <t>RM Quantitative Test-5</t>
-  </si>
-  <si>
-    <t>RM Quantitative Test-6</t>
-  </si>
-  <si>
-    <t>SMAUTO8</t>
-  </si>
-  <si>
-    <t>SM008</t>
-  </si>
-  <si>
-    <t>SMAUTO9</t>
-  </si>
-  <si>
-    <t>SM009</t>
-  </si>
-  <si>
-    <t>REGAUTO5</t>
-  </si>
-  <si>
-    <t>REG005</t>
   </si>
   <si>
     <t>REGAUTO6</t>
@@ -2862,7 +2880,7 @@
     </row>
     <row r="2" spans="1:2">
       <c r="A2" s="1" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>193</v>
@@ -2870,7 +2888,7 @@
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="1" t="s">
-        <v>212</v>
+        <v>208</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>193</v>
@@ -2878,7 +2896,7 @@
     </row>
     <row r="4" spans="1:2">
       <c r="A4" s="1" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>193</v>
@@ -2886,7 +2904,7 @@
     </row>
     <row r="5" spans="1:2">
       <c r="A5" s="1" t="s">
-        <v>215</v>
+        <v>211</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>193</v>
@@ -2894,7 +2912,7 @@
     </row>
     <row r="6" spans="1:2">
       <c r="A6" s="1" t="s">
-        <v>216</v>
+        <v>212</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>193</v>
@@ -2902,7 +2920,7 @@
     </row>
     <row r="7" spans="1:2">
       <c r="A7" s="1" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>193</v>
@@ -2910,7 +2928,7 @@
     </row>
     <row r="8" spans="1:2">
       <c r="A8" s="1" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
       <c r="B8" s="7" t="s">
         <v>200</v>
@@ -2918,7 +2936,7 @@
     </row>
     <row r="9" spans="1:2">
       <c r="A9" s="1" t="s">
-        <v>219</v>
+        <v>215</v>
       </c>
       <c r="B9" s="7" t="s">
         <v>200</v>
@@ -2926,7 +2944,7 @@
     </row>
     <row r="10" spans="1:2">
       <c r="A10" s="1" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="B10" s="7" t="s">
         <v>200</v>
@@ -2934,7 +2952,7 @@
     </row>
     <row r="11" spans="1:2">
       <c r="A11" s="1" t="s">
-        <v>221</v>
+        <v>217</v>
       </c>
       <c r="B11" s="7" t="s">
         <v>200</v>
@@ -2942,7 +2960,7 @@
     </row>
     <row r="12" spans="1:2">
       <c r="A12" s="1" t="s">
-        <v>222</v>
+        <v>218</v>
       </c>
       <c r="B12" s="7" t="s">
         <v>200</v>
@@ -2950,7 +2968,7 @@
     </row>
     <row r="13" spans="1:2">
       <c r="A13" s="1" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
       <c r="B13" s="7" t="s">
         <v>200</v>
@@ -3029,7 +3047,7 @@
   <dimension ref="A1:J9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J13" sqref="J13"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3065,7 +3083,7 @@
         <v>137</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>211</v>
+        <v>226</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>119</v>
@@ -3077,147 +3095,147 @@
         <v>139</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>208</v>
+        <v>227</v>
       </c>
     </row>
     <row r="3" spans="1:6">
-      <c r="A3" s="1" t="s">
-        <v>224</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>211</v>
-      </c>
-      <c r="C3" s="1" t="s">
+      <c r="A3" t="s">
+        <v>228</v>
+      </c>
+      <c r="B3" t="s">
+        <v>226</v>
+      </c>
+      <c r="C3" t="s">
         <v>119</v>
       </c>
-      <c r="D3" s="1">
+      <c r="D3">
         <v>8</v>
       </c>
-      <c r="E3" s="3" t="s">
-        <v>225</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>208</v>
+      <c r="E3" t="s">
+        <v>229</v>
+      </c>
+      <c r="F3" t="s">
+        <v>227</v>
       </c>
     </row>
     <row r="4" spans="1:6">
-      <c r="A4" s="1" t="s">
+      <c r="A4" t="s">
+        <v>230</v>
+      </c>
+      <c r="B4" t="s">
         <v>226</v>
       </c>
-      <c r="B4" s="1" t="s">
-        <v>211</v>
-      </c>
-      <c r="C4" s="1" t="s">
+      <c r="C4" t="s">
         <v>119</v>
       </c>
-      <c r="D4" s="1">
+      <c r="D4">
         <v>9</v>
       </c>
-      <c r="E4" s="1" t="s">
+      <c r="E4" t="s">
+        <v>231</v>
+      </c>
+      <c r="F4" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5" t="s">
+        <v>233</v>
+      </c>
+      <c r="B5" t="s">
+        <v>226</v>
+      </c>
+      <c r="C5" t="s">
+        <v>191</v>
+      </c>
+      <c r="D5">
+        <v>5</v>
+      </c>
+      <c r="E5" t="s">
+        <v>234</v>
+      </c>
+      <c r="F5" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6" t="s">
+        <v>236</v>
+      </c>
+      <c r="B6" t="s">
+        <v>226</v>
+      </c>
+      <c r="C6" t="s">
+        <v>191</v>
+      </c>
+      <c r="D6">
+        <v>6</v>
+      </c>
+      <c r="E6" t="s">
+        <v>237</v>
+      </c>
+      <c r="F6" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7" t="s">
+        <v>167</v>
+      </c>
+      <c r="B7" t="s">
+        <v>226</v>
+      </c>
+      <c r="C7" t="s">
+        <v>155</v>
+      </c>
+      <c r="D7">
+        <v>7</v>
+      </c>
+      <c r="E7" t="s">
+        <v>168</v>
+      </c>
+      <c r="F7" t="s">
         <v>227</v>
       </c>
-      <c r="F4" s="1" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6">
-      <c r="A5" s="1" t="s">
-        <v>228</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>211</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>191</v>
-      </c>
-      <c r="D5" s="1">
-        <v>5</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>229</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6">
-      <c r="A6" s="1" t="s">
-        <v>230</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>211</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>191</v>
-      </c>
-      <c r="D6" s="1">
-        <v>6</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>231</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6">
-      <c r="A7" s="1" t="s">
-        <v>167</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>211</v>
-      </c>
-      <c r="C7" s="1" t="s">
+    </row>
+    <row r="8" spans="1:6">
+      <c r="A8" t="s">
+        <v>238</v>
+      </c>
+      <c r="B8" t="s">
+        <v>226</v>
+      </c>
+      <c r="C8" t="s">
         <v>155</v>
       </c>
-      <c r="D7" s="1">
-        <v>7</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>168</v>
-      </c>
-      <c r="F7" s="1" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6">
-      <c r="A8" s="1" t="s">
+      <c r="D8">
+        <v>8</v>
+      </c>
+      <c r="E8" t="s">
+        <v>239</v>
+      </c>
+      <c r="F8" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="A9" t="s">
+        <v>240</v>
+      </c>
+      <c r="B9" t="s">
+        <v>226</v>
+      </c>
+      <c r="C9" t="s">
+        <v>155</v>
+      </c>
+      <c r="D9">
+        <v>9</v>
+      </c>
+      <c r="E9" t="s">
+        <v>241</v>
+      </c>
+      <c r="F9" t="s">
         <v>232</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>211</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>155</v>
-      </c>
-      <c r="D8" s="1">
-        <v>8</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>233</v>
-      </c>
-      <c r="F8" s="1" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6">
-      <c r="A9" s="1" t="s">
-        <v>234</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>211</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>155</v>
-      </c>
-      <c r="D9" s="1">
-        <v>9</v>
-      </c>
-      <c r="E9" s="3" t="s">
-        <v>235</v>
-      </c>
-      <c r="F9" s="1" t="s">
-        <v>210</v>
       </c>
     </row>
   </sheetData>
@@ -3428,13 +3446,45 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E14" sqref="E14"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="14" customWidth="1"/>
+    <col min="2" max="2" width="19" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>225</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>